<commit_message>
adding title and bullet points
</commit_message>
<xml_diff>
--- a/welcome-paragraph.xlsx
+++ b/welcome-paragraph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training Rony\web0\GP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ADCC59-FA7C-4DE4-8CB3-BC1150D2978C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A987F2-23C8-4831-A3F2-0C2C58050133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>At Powerful Digital Solutions, we help businesses of all sizes reach their full digital potential. Our team of talented digital marketers specializes in a range of services, including SEO, PPC, social media marketing, content creation, email marketing, and more. We are passionate about using the latest technologies and strategies to help our clients achieve their goals and drive results. Whether you are looking to increase your online visibility, generate leads, or boost your revenue, we have the expertise and experience to make it happen. Let us help you take your business to the next level with our powerful digital solutions.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Digital Marketing Solutions for Business Growth</t>
+  </si>
+  <si>
+    <t>Powerful Digital Solutions is a leading digital marketing agency that helps businesses of all sizes achieve their digital potential. We specialize in providing a wide range of services, from SEO to social media marketing, to help our clients achieve their marketing goals and drive growth.</t>
+  </si>
+  <si>
+    <t>Our team of talented digital marketers is passionate about using the latest technologies and strategies to deliver the best results for our clients.</t>
+  </si>
+  <si>
+    <t>We take a personalized approach to every project, working closely with our clients to understand their business needs and objectives.</t>
+  </si>
+  <si>
+    <t>Whether you're looking to increase your online visibility, generate leads, or boost your revenue, we have the expertise and experience to help you succeed.</t>
+  </si>
+  <si>
+    <t>At Powerful Digital Solutions, we believe that digital marketing is key to unlocking business growth in today's digital age. Let us help you take your business to the next level with our powerful digital solutions. Contact us today to learn more.</t>
   </si>
 </sst>
 </file>
@@ -348,26 +363,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="85.85546875" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="55.140625" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>